<commit_message>
Cleaned up documentation working files.
</commit_message>
<xml_diff>
--- a/docs/Figures/RenalWorking.xlsx
+++ b/docs/Figures/RenalWorking.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\docs\Figures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10296" yWindow="12" windowWidth="5076" windowHeight="8136" activeTab="3"/>
+    <workbookView xWindow="10290" yWindow="15" windowWidth="5070" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="MolecularRadius" sheetId="1" r:id="rId1"/>
     <sheet name="Filterability" sheetId="2" r:id="rId2"/>
-    <sheet name="RenalNodesandPaths" sheetId="3" r:id="rId3"/>
-    <sheet name="RenalAutoRegulation_MAP" sheetId="4" r:id="rId4"/>
+    <sheet name="RenalAutoRegulation_MAP" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="HighMAP_RBF_GFR" localSheetId="3">RenalAutoRegulation_MAP!$K$2:$L$29</definedName>
-    <definedName name="LowMAP_GFR" localSheetId="3">RenalAutoRegulation_MAP!$A$2:$B$7</definedName>
-    <definedName name="LowMAP_GFR_1" localSheetId="3">RenalAutoRegulation_MAP!$V$2:$W$7</definedName>
-    <definedName name="LowMAP_RBF" localSheetId="3">RenalAutoRegulation_MAP!$C$2:$D$23</definedName>
-    <definedName name="LowMAP_RBF_1" localSheetId="3">RenalAutoRegulation_MAP!$P$2:$Q$23</definedName>
-    <definedName name="NormalMAP_RBF_GFR" localSheetId="3">RenalAutoRegulation_MAP!$F$2:$G$24</definedName>
+    <definedName name="HighMAP_RBF_GFR" localSheetId="2">RenalAutoRegulation_MAP!$K$2:$L$29</definedName>
+    <definedName name="LowMAP_GFR" localSheetId="2">RenalAutoRegulation_MAP!$A$2:$B$7</definedName>
+    <definedName name="LowMAP_GFR_1" localSheetId="2">RenalAutoRegulation_MAP!$V$2:$W$7</definedName>
+    <definedName name="LowMAP_RBF" localSheetId="2">RenalAutoRegulation_MAP!$C$2:$D$23</definedName>
+    <definedName name="LowMAP_RBF_1" localSheetId="2">RenalAutoRegulation_MAP!$P$2:$Q$23</definedName>
+    <definedName name="NormalMAP_RBF_GFR" localSheetId="2">RenalAutoRegulation_MAP!$F$2:$G$24</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -78,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Filterability</t>
   </si>
@@ -170,250 +174,6 @@
     <t>Polyanionic Dextran (Negative)</t>
   </si>
   <si>
-    <t>Nodes</t>
-  </si>
-  <si>
-    <t>Node</t>
-  </si>
-  <si>
-    <t>Node Enum</t>
-  </si>
-  <si>
-    <t>Mapped to Compartment
-(None if Blank)</t>
-  </si>
-  <si>
-    <t>RightRenalAortaConnectionNode</t>
-  </si>
-  <si>
-    <t>RightRenalArteryNode</t>
-  </si>
-  <si>
-    <t>RightRenalArtery</t>
-  </si>
-  <si>
-    <t>RightAfferentArterioleNode</t>
-  </si>
-  <si>
-    <t>RightAfferentArteriole</t>
-  </si>
-  <si>
-    <t>RightGlomerularCapillariesNode</t>
-  </si>
-  <si>
-    <t>RightGlomerularCapillaries, RightKidney, RightNephron</t>
-  </si>
-  <si>
-    <t>RightEfferentArterioleNode</t>
-  </si>
-  <si>
-    <t>RightEfferentArteriole</t>
-  </si>
-  <si>
-    <t>RightPeritubularCapillariesNode</t>
-  </si>
-  <si>
-    <t>RightPeritubularCapillaries</t>
-  </si>
-  <si>
-    <t>RightRenalVeinNode</t>
-  </si>
-  <si>
-    <t>RightRenalVein</t>
-  </si>
-  <si>
-    <t>RightRenalVenaCavaConnectionNode</t>
-  </si>
-  <si>
-    <t>RightNetGlomerularCapillariesNode</t>
-  </si>
-  <si>
-    <t>RightGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>RightNetBowmansCapsulesNode</t>
-  </si>
-  <si>
-    <t>RightBowmansCapsules</t>
-  </si>
-  <si>
-    <t>RightBowmansCapsulesNode</t>
-  </si>
-  <si>
-    <t>RightTubulesNode</t>
-  </si>
-  <si>
-    <t>RightTubules</t>
-  </si>
-  <si>
-    <t>RightNetTubulesNode</t>
-  </si>
-  <si>
-    <t>RightNetPeritubularCapillariesNode</t>
-  </si>
-  <si>
-    <t>RightUreterNode</t>
-  </si>
-  <si>
-    <t>RightUreter</t>
-  </si>
-  <si>
-    <t>LeftRenalAortaConnectionNode</t>
-  </si>
-  <si>
-    <t>LeftRenalArteryNode</t>
-  </si>
-  <si>
-    <t>LeftRenalArtery</t>
-  </si>
-  <si>
-    <t>LeftAfferentArterioleNode</t>
-  </si>
-  <si>
-    <t>LeftAfferentArteriole</t>
-  </si>
-  <si>
-    <t>LeftGlomerularCapillariesNode</t>
-  </si>
-  <si>
-    <t>LeftGlomerularCapillaries, LeftKidney, LeftNephron</t>
-  </si>
-  <si>
-    <t>LeftEfferentArterioleNode</t>
-  </si>
-  <si>
-    <t>LeftEfferentArteriole</t>
-  </si>
-  <si>
-    <t>LeftPeritubularCapillariesNode</t>
-  </si>
-  <si>
-    <t>LeftPeritubularCapillaries</t>
-  </si>
-  <si>
-    <t>LeftRenalVeinNode</t>
-  </si>
-  <si>
-    <t>LeftRenalVein</t>
-  </si>
-  <si>
-    <t>LeftRenalVenaCavaConnectionNode</t>
-  </si>
-  <si>
-    <t>LeftNetGlomerularCapillariesNode</t>
-  </si>
-  <si>
-    <t>LeftGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>LeftNetBowmansCapsulesNode</t>
-  </si>
-  <si>
-    <t>LeftBowmansCapsules</t>
-  </si>
-  <si>
-    <t>LeftBowmansCapsulesNode</t>
-  </si>
-  <si>
-    <t>LeftTubulesNode</t>
-  </si>
-  <si>
-    <t>LeftTubules</t>
-  </si>
-  <si>
-    <t>LeftNetTubulesNode</t>
-  </si>
-  <si>
-    <t>LeftNetPeritubularCapillariesNode</t>
-  </si>
-  <si>
-    <t>LeftUreterNode</t>
-  </si>
-  <si>
-    <t>LeftUreter</t>
-  </si>
-  <si>
-    <t>BladderNode</t>
-  </si>
-  <si>
-    <t>Bladder</t>
-  </si>
-  <si>
-    <t>RenalGround (equivalent to Cardiovascular Ground)</t>
-  </si>
-  <si>
-    <t>Urethra</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Paths</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Path Element</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>RightRenalArtery, RightAfferentArteriole</t>
-  </si>
-  <si>
-    <t>RightAfferentArteriole, RightGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>RightEfferentArteriole, RightGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>RenalGround</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>Voltage Source</t>
-  </si>
-  <si>
-    <t>RightBowmansCapsules, RightTubules</t>
-  </si>
-  <si>
-    <t>RightTubules, RightUreter</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>LeftRenalArtery, LeftAfferentArteriole</t>
-  </si>
-  <si>
-    <t>LeftAfferentArteriole, LeftGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>LeftEfferentArteriole, LeftGlomerularCapillaries</t>
-  </si>
-  <si>
-    <t>LeftBowmansCapsules, LeftTubules</t>
-  </si>
-  <si>
-    <t>LeftTubules, LeftUreter</t>
-  </si>
-  <si>
-    <t>Bladder, Urethra</t>
-  </si>
-  <si>
     <t>MAP (mmHg)</t>
   </si>
   <si>
@@ -444,8 +204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,31 +341,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,18 +524,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -913,293 +644,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1245,84 +689,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1375,12 +747,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1479,6 +854,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8EF-48AE-84CB-4207818EFBE7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1540,7 +920,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1654,6 +1034,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9C56-48BA-8E1B-17642611E287}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1754,7 +1139,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2003,6 +1388,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BBA0-4CBA-A359-8260746CC205}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2234,6 +1624,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BBA0-4CBA-A359-8260746CC205}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2465,6 +1860,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BBA0-4CBA-A359-8260746CC205}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2599,7 +1999,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2633,7 +2033,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3022,6 +2421,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9CF8-4BFD-AE53-455C5DF622CF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3140,6 +2544,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9CF8-4BFD-AE53-455C5DF622CF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3179,7 +2588,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3246,7 +2654,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3280,7 +2688,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3453,6 +2860,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A56-4FC8-8051-731748888CD5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3571,6 +2983,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A56-4FC8-8051-731748888CD5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3611,7 +3028,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3647,7 +3063,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3688,7 +3103,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3718,7 +3139,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3753,7 +3180,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3788,7 +3221,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3818,7 +3257,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3841,23 +3286,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NormalMAP_RBF_GFR" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LowMAP_RBF_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="HighMAP_RBF_GFR" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LowMAP_RBF" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LowMAP_GFR" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NormalMAP_RBF_GFR" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3903,7 +3348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3936,9 +3381,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3971,6 +3433,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4149,15 +3628,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="7" width="26.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4378,11 +3857,11 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4392,11 +3871,11 @@
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -4619,1198 +4098,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
-  <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="26.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
-        <v>14</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>15</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
-        <v>16</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>17</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
-        <v>18</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>19</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
-        <v>20</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
-        <v>21</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
-        <v>22</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
-        <v>23</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
-        <v>24</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
-        <v>25</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="6">
-        <v>26</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="6">
-        <v>27</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
-        <v>28</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
-        <v>32</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="13">
-        <v>32</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-    </row>
-    <row r="43" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="6">
-        <v>1</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="6">
-        <v>2</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="6">
-        <v>3</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="6">
-        <v>4</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="6">
-        <v>5</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="6">
-        <v>6</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="6">
-        <v>7</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="6">
-        <v>8</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="6">
-        <v>9</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="6">
-        <v>10</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="6">
-        <v>11</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="6">
-        <v>12</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="6">
-        <v>13</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="6">
-        <v>14</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="6">
-        <v>15</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="6">
-        <v>16</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="6">
-        <v>17</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="6">
-        <v>18</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="6">
-        <v>19</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="6">
-        <v>20</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="6">
-        <v>21</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="6">
-        <v>22</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="6">
-        <v>23</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="6">
-        <v>24</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="6">
-        <v>25</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="6">
-        <v>26</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="6">
-        <v>27</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="6">
-        <v>28</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E71" s="9"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="6">
-        <v>29</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E72" s="9"/>
-    </row>
-    <row r="73" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="6">
-        <v>30</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="6">
-        <v>31</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E74" s="9"/>
-    </row>
-    <row r="75" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="6">
-        <v>32</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="6">
-        <v>33</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="6">
-        <v>34</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="6">
-        <v>35</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="6">
-        <v>36</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="6">
-        <v>37</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="6">
-        <v>38</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="6">
-        <v>39</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="6">
-        <v>40</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="11">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A35:B35"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="15"/>
+    <col min="5" max="5" width="8.85546875" style="2"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="15"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="2"/>
     <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="11.77734375" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
     <col min="20" max="20" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>49.010501258415204</v>
       </c>
@@ -5869,7 +4238,7 @@
         <v>-6.3828198875230903E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>55.7918097623268</v>
       </c>
@@ -5928,7 +4297,7 @@
         <v>3.0570347882347301E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>63.412227085063897</v>
       </c>
@@ -5987,7 +4356,7 @@
         <v>5.6904145722391303E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>71.877704353000894</v>
       </c>
@@ -6046,7 +4415,7 @@
         <v>8.3219280346389299E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>76.120857458125101</v>
       </c>
@@ -6105,7 +4474,7 @@
         <v>0.114928084407505</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>79.504072802112603</v>
       </c>
@@ -6164,7 +4533,7 @@
         <v>0.120153784900214</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>54.712448495442601</v>
       </c>
@@ -6217,7 +4586,7 @@
         <v>0.123189843285062</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>56.417530278436701</v>
       </c>
@@ -6264,7 +4633,7 @@
         <v>0.122297163261257</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>58.134598576601299</v>
       </c>
@@ -6311,7 +4680,7 @@
         <v>0.12185082324935501</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>60.693719565488799</v>
       </c>
@@ -6352,7 +4721,7 @@
         <v>0.121181313231502</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>61.559745286552598</v>
       </c>
@@ -6393,7 +4762,7 @@
         <v>0.12058619321563201</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>63.273816955924502</v>
       </c>
@@ -6434,7 +4803,7 @@
         <v>0.12010265820273799</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>64.990885254089093</v>
       </c>
@@ -6475,7 +4844,7 @@
         <v>0.11984229319579399</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>66.704956923461097</v>
       </c>
@@ -6516,7 +4885,7 @@
         <v>0.124566058321761</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>67.567986015732302</v>
       </c>
@@ -6551,7 +4920,7 @@
         <v>0.124119718309859</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>68.437008365588696</v>
       </c>
@@ -6577,7 +4946,7 @@
         <v>0.12190812720848</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>70.157073292545803</v>
       </c>
@@ -6605,7 +4974,7 @@
         <v>0.12190812720848</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>71.023099013609595</v>
       </c>
@@ -6633,7 +5002,7 @@
         <v>0.13250883392226101</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>72.731177425396396</v>
       </c>
@@ -6661,7 +5030,7 @@
         <v>0.13780918727915101</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>75.293295043076498</v>
       </c>
@@ -6689,7 +5058,7 @@
         <v>0.148409893992932</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>77.852416031963998</v>
       </c>
@@ -6717,7 +5086,7 @@
         <v>0.153710247349823</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>79.551504557372894</v>
       </c>
@@ -6733,25 +5102,25 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="F24" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="K24" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="K24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
       <c r="P24" s="1">
         <v>81.640466154227596</v>
       </c>
@@ -6761,7 +5130,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P25" s="1">
         <v>90.096702206793907</v>
       </c>
@@ -6771,7 +5140,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P26" s="1">
         <v>101.933052318373</v>
       </c>
@@ -6781,7 +5150,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P27" s="1">
         <v>108.69328043639899</v>
       </c>
@@ -6791,7 +5160,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P28" s="1">
         <v>118.83957351847199</v>
       </c>
@@ -6801,7 +5170,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P29" s="1">
         <v>125.599801636498</v>
       </c>
@@ -6811,7 +5180,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P30" s="1">
         <v>134.05603768906499</v>
       </c>
@@ -6821,7 +5190,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P31" s="1">
         <v>141.661294321844</v>
       </c>
@@ -6831,7 +5200,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P32" s="1">
         <v>146.73741631539701</v>
       </c>
@@ -6841,7 +5210,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P33" s="1">
         <v>151.813538308951</v>
       </c>
@@ -6849,7 +5218,7 @@
         <v>1.2345764729220301</v>
       </c>
     </row>
-    <row r="34" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P34" s="1">
         <v>156.88966030250401</v>
       </c>
@@ -6857,7 +5226,7 @@
         <v>1.2396349930569299</v>
       </c>
     </row>
-    <row r="35" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P35" s="1">
         <v>162.80485990577699</v>
       </c>
@@ -6865,7 +5234,7 @@
         <v>1.23937462804999</v>
       </c>
     </row>
-    <row r="36" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P36" s="1">
         <v>169.582940738904</v>
       </c>
@@ -6873,7 +5242,7 @@
         <v>1.2549221384645901</v>
       </c>
     </row>
-    <row r="37" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P37" s="1">
         <v>177.20009918175001</v>
       </c>
@@ -6881,7 +5250,7 @@
         <v>1.26515076373735</v>
       </c>
     </row>
-    <row r="38" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P38" s="1">
         <v>178.09187279151899</v>
       </c>
@@ -6889,7 +5258,7 @@
         <v>1.27208480565371</v>
       </c>
     </row>
-    <row r="39" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P39" s="1">
         <v>182.33215547703099</v>
       </c>
@@ -6897,7 +5266,7 @@
         <v>1.2879858657243799</v>
       </c>
     </row>
-    <row r="40" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P40" s="1">
         <v>187.42049469964601</v>
       </c>
@@ -6905,7 +5274,7 @@
         <v>1.3144876325088299</v>
       </c>
     </row>
-    <row r="41" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P41" s="1">
         <v>191.66077738515901</v>
       </c>
@@ -6913,7 +5282,7 @@
         <v>1.3303886925795001</v>
       </c>
     </row>
-    <row r="42" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P42" s="1">
         <v>195.05300353356799</v>
       </c>
@@ -6921,7 +5290,7 @@
         <v>1.3568904593639499</v>
       </c>
     </row>
-    <row r="43" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P43" s="1">
         <v>197.597173144876</v>
       </c>
@@ -6929,7 +5298,7 @@
         <v>1.3780918727915099</v>
       </c>
     </row>
-    <row r="44" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P44" s="1">
         <v>200.989399293286</v>
       </c>
@@ -6937,7 +5306,7 @@
         <v>1.4045936395759699</v>
       </c>
     </row>
-    <row r="45" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P45" s="1">
         <v>204.381625441696</v>
       </c>
@@ -6945,7 +5314,7 @@
         <v>1.43639575971731</v>
       </c>
     </row>
-    <row r="46" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P46" s="1">
         <v>206.07773851590099</v>
       </c>
@@ -6953,7 +5322,7 @@
         <v>1.4469964664310899</v>
       </c>
     </row>
-    <row r="47" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P47" s="1">
         <v>209.46996466431</v>
       </c>
@@ -6961,7 +5330,7 @@
         <v>1.47349823321554</v>
       </c>
     </row>
-    <row r="48" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P48" s="1">
         <v>212.01413427561801</v>
       </c>
@@ -6969,7 +5338,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P49" s="1">
         <v>214.55830388692499</v>
       </c>
@@ -6977,7 +5346,7 @@
         <v>1.5318021201413401</v>
       </c>
     </row>
-    <row r="50" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P50" s="1">
         <v>218.79858657243801</v>
       </c>
@@ -6985,7 +5354,7 @@
         <v>1.5742049469964601</v>
       </c>
     </row>
-    <row r="51" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P51" s="1">
         <v>221.342756183745</v>
       </c>
@@ -6993,7 +5362,7 @@
         <v>1.6060070671377999</v>
       </c>
     </row>
-    <row r="52" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P52" s="1">
         <v>223.03886925795001</v>
       </c>
@@ -7001,7 +5370,7 @@
         <v>1.63780918727915</v>
       </c>
     </row>
-    <row r="53" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P53" s="1">
         <v>226.43109540635999</v>
       </c>
@@ -7009,7 +5378,7 @@
         <v>1.6643109540636001</v>
       </c>
     </row>
-    <row r="54" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P54" s="1">
         <v>227.27915194346201</v>
       </c>
@@ -7017,7 +5386,7 @@
         <v>1.6908127208480499</v>
       </c>
     </row>
-    <row r="55" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P55" s="1">
         <v>228.975265017667</v>
       </c>
@@ -7025,7 +5394,7 @@
         <v>1.7173144876324999</v>
       </c>
     </row>
-    <row r="56" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P56" s="1">
         <v>230.67137809187199</v>
       </c>
@@ -7033,7 +5402,7 @@
         <v>1.74911660777385</v>
       </c>
     </row>
-    <row r="57" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P57" s="1">
         <v>232.367491166077</v>
       </c>
@@ -7041,7 +5410,7 @@
         <v>1.77031802120141</v>
       </c>
     </row>
-    <row r="58" spans="16:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P58" s="1">
         <v>234.06360424028199</v>
       </c>
@@ -7061,21 +5430,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D00DDCF912707249810263345C6FBCAE" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05fc12c866532ec63d2052ef81b63530">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="711b5f35d88f7f6ebfe284b0f73f4393">
     <xsd:element name="properties">
@@ -7189,17 +5543,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32A4371-0319-413F-ADEF-5CE307745E9E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{940FFB9C-3869-462C-A17A-AFAAE045C4A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7213,17 +5583,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{940FFB9C-3869-462C-A17A-AFAAE045C4A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32A4371-0319-413F-ADEF-5CE307745E9E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>